<commit_message>
Improved taxa map, fixed station issue
</commit_message>
<xml_diff>
--- a/Data/zoop_stations.xlsx
+++ b/Data/zoop_stations.xlsx
@@ -1999,8 +1999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G431"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A397" workbookViewId="0">
-      <selection activeCell="C418" sqref="C418"/>
+    <sheetView tabSelected="1" topLeftCell="A406" workbookViewId="0">
+      <selection activeCell="D342" sqref="D342"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6712,7 +6712,7 @@
         <v>38.008040000000001</v>
       </c>
       <c r="D343" s="30">
-        <v>-21.456099999999999</v>
+        <v>-121.45610000000001</v>
       </c>
     </row>
     <row r="344" spans="1:4">

</xml_diff>

<commit_message>
Finished integrating all zoop datasets by adding Micro and Macrozoops to integrated dataset.
</commit_message>
<xml_diff>
--- a/Data/zoop_stations.xlsx
+++ b/Data/zoop_stations.xlsx
@@ -781,9 +781,6 @@
     <t>LonS</t>
   </si>
   <si>
-    <t>20mm</t>
-  </si>
-  <si>
     <t>501 FRP</t>
   </si>
   <si>
@@ -1373,6 +1370,9 @@
   </si>
   <si>
     <t>YBFMP</t>
+  </si>
+  <si>
+    <t>twentymm</t>
   </si>
 </sst>
 </file>
@@ -1999,8 +1999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G431"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A406" workbookViewId="0">
-      <selection activeCell="D342" sqref="D342"/>
+    <sheetView tabSelected="1" topLeftCell="A144" workbookViewId="0">
+      <selection activeCell="L169" sqref="L169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2019,10 +2019,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="29" t="s">
+        <v>392</v>
+      </c>
+      <c r="D1" s="29" t="s">
         <v>393</v>
-      </c>
-      <c r="D1" s="29" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -4365,7 +4365,7 @@
     </row>
     <row r="172" spans="1:4">
       <c r="A172" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B172" s="33">
         <v>997</v>
@@ -4373,7 +4373,7 @@
     </row>
     <row r="173" spans="1:4">
       <c r="A173" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B173" s="33">
         <v>998</v>
@@ -4381,7 +4381,7 @@
     </row>
     <row r="174" spans="1:4">
       <c r="A174" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B174" s="33">
         <v>999</v>
@@ -4389,7 +4389,7 @@
     </row>
     <row r="175" spans="1:4">
       <c r="A175" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B175" s="33">
         <v>323</v>
@@ -4403,7 +4403,7 @@
     </row>
     <row r="176" spans="1:4">
       <c r="A176" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B176" s="33">
         <v>328</v>
@@ -4417,7 +4417,7 @@
     </row>
     <row r="177" spans="1:4">
       <c r="A177" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B177" s="33">
         <v>329</v>
@@ -4431,7 +4431,7 @@
     </row>
     <row r="178" spans="1:4">
       <c r="A178" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B178" s="33">
         <v>334</v>
@@ -4445,7 +4445,7 @@
     </row>
     <row r="179" spans="1:4">
       <c r="A179" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B179" s="33">
         <v>335</v>
@@ -4459,7 +4459,7 @@
     </row>
     <row r="180" spans="1:4">
       <c r="A180" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B180" s="33">
         <v>336</v>
@@ -4473,7 +4473,7 @@
     </row>
     <row r="181" spans="1:4">
       <c r="A181" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B181" s="33">
         <v>340</v>
@@ -4487,7 +4487,7 @@
     </row>
     <row r="182" spans="1:4">
       <c r="A182" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B182" s="33">
         <v>341</v>
@@ -4501,7 +4501,7 @@
     </row>
     <row r="183" spans="1:4">
       <c r="A183" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B183" s="33">
         <v>342</v>
@@ -4515,7 +4515,7 @@
     </row>
     <row r="184" spans="1:4">
       <c r="A184" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B184" s="33">
         <v>343</v>
@@ -4529,7 +4529,7 @@
     </row>
     <row r="185" spans="1:4">
       <c r="A185" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B185" s="33">
         <v>344</v>
@@ -4543,7 +4543,7 @@
     </row>
     <row r="186" spans="1:4">
       <c r="A186" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B186" s="33">
         <v>345</v>
@@ -4557,7 +4557,7 @@
     </row>
     <row r="187" spans="1:4">
       <c r="A187" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B187" s="33">
         <v>346</v>
@@ -4571,7 +4571,7 @@
     </row>
     <row r="188" spans="1:4">
       <c r="A188" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B188" s="33">
         <v>405</v>
@@ -4585,7 +4585,7 @@
     </row>
     <row r="189" spans="1:4">
       <c r="A189" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B189" s="33">
         <v>411</v>
@@ -4599,7 +4599,7 @@
     </row>
     <row r="190" spans="1:4">
       <c r="A190" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B190" s="33">
         <v>418</v>
@@ -4613,7 +4613,7 @@
     </row>
     <row r="191" spans="1:4">
       <c r="A191" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B191" s="33">
         <v>501</v>
@@ -4627,7 +4627,7 @@
     </row>
     <row r="192" spans="1:4">
       <c r="A192" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B192" s="33">
         <v>504</v>
@@ -4641,7 +4641,7 @@
     </row>
     <row r="193" spans="1:7">
       <c r="A193" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B193" s="33">
         <v>508</v>
@@ -4655,7 +4655,7 @@
     </row>
     <row r="194" spans="1:7">
       <c r="A194" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B194" s="33">
         <v>513</v>
@@ -4669,7 +4669,7 @@
     </row>
     <row r="195" spans="1:7">
       <c r="A195" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B195" s="33">
         <v>519</v>
@@ -4683,7 +4683,7 @@
     </row>
     <row r="196" spans="1:7">
       <c r="A196" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B196" s="33">
         <v>520</v>
@@ -4697,7 +4697,7 @@
     </row>
     <row r="197" spans="1:7">
       <c r="A197" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B197" s="33">
         <v>602</v>
@@ -4711,7 +4711,7 @@
     </row>
     <row r="198" spans="1:7">
       <c r="A198" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B198" s="33">
         <v>606</v>
@@ -4725,7 +4725,7 @@
     </row>
     <row r="199" spans="1:7">
       <c r="A199" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B199" s="33">
         <v>609</v>
@@ -4739,7 +4739,7 @@
     </row>
     <row r="200" spans="1:7">
       <c r="A200" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B200" s="33">
         <v>610</v>
@@ -4753,7 +4753,7 @@
     </row>
     <row r="201" spans="1:7">
       <c r="A201" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B201" s="33">
         <v>703</v>
@@ -4767,7 +4767,7 @@
     </row>
     <row r="202" spans="1:7">
       <c r="A202" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B202" s="33">
         <v>704</v>
@@ -4783,7 +4783,7 @@
     </row>
     <row r="203" spans="1:7">
       <c r="A203" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B203" s="33">
         <v>705</v>
@@ -4797,7 +4797,7 @@
     </row>
     <row r="204" spans="1:7">
       <c r="A204" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B204" s="33">
         <v>706</v>
@@ -4811,7 +4811,7 @@
     </row>
     <row r="205" spans="1:7">
       <c r="A205" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B205" s="33">
         <v>707</v>
@@ -4825,7 +4825,7 @@
     </row>
     <row r="206" spans="1:7">
       <c r="A206" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B206" s="33">
         <v>711</v>
@@ -4839,7 +4839,7 @@
     </row>
     <row r="207" spans="1:7">
       <c r="A207" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B207" s="33">
         <v>716</v>
@@ -4853,7 +4853,7 @@
     </row>
     <row r="208" spans="1:7">
       <c r="A208" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B208" s="33">
         <v>801</v>
@@ -4867,7 +4867,7 @@
     </row>
     <row r="209" spans="1:4">
       <c r="A209" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B209" s="33">
         <v>802</v>
@@ -4881,7 +4881,7 @@
     </row>
     <row r="210" spans="1:4">
       <c r="A210" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B210" s="33">
         <v>804</v>
@@ -4895,7 +4895,7 @@
     </row>
     <row r="211" spans="1:4">
       <c r="A211" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B211" s="33">
         <v>809</v>
@@ -4909,7 +4909,7 @@
     </row>
     <row r="212" spans="1:4">
       <c r="A212" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B212" s="33">
         <v>812</v>
@@ -4923,7 +4923,7 @@
     </row>
     <row r="213" spans="1:4">
       <c r="A213" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B213" s="33">
         <v>815</v>
@@ -4937,7 +4937,7 @@
     </row>
     <row r="214" spans="1:4">
       <c r="A214" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B214" s="33">
         <v>901</v>
@@ -4951,7 +4951,7 @@
     </row>
     <row r="215" spans="1:4">
       <c r="A215" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B215" s="33">
         <v>902</v>
@@ -4965,7 +4965,7 @@
     </row>
     <row r="216" spans="1:4">
       <c r="A216" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B216" s="33">
         <v>906</v>
@@ -4979,7 +4979,7 @@
     </row>
     <row r="217" spans="1:4">
       <c r="A217" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B217" s="33">
         <v>910</v>
@@ -4993,7 +4993,7 @@
     </row>
     <row r="218" spans="1:4">
       <c r="A218" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B218" s="33">
         <v>912</v>
@@ -5007,7 +5007,7 @@
     </row>
     <row r="219" spans="1:4">
       <c r="A219" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B219" s="33">
         <v>914</v>
@@ -5021,7 +5021,7 @@
     </row>
     <row r="220" spans="1:4">
       <c r="A220" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B220" s="33">
         <v>915</v>
@@ -5035,7 +5035,7 @@
     </row>
     <row r="221" spans="1:4">
       <c r="A221" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B221" s="33">
         <v>918</v>
@@ -5049,7 +5049,7 @@
     </row>
     <row r="222" spans="1:4">
       <c r="A222" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B222" s="33">
         <v>919</v>
@@ -5063,7 +5063,7 @@
     </row>
     <row r="223" spans="1:4">
       <c r="A223" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B223" s="33">
         <v>330</v>
@@ -5077,7 +5077,7 @@
     </row>
     <row r="224" spans="1:4">
       <c r="A224" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B224" s="33">
         <v>347</v>
@@ -5091,7 +5091,7 @@
     </row>
     <row r="225" spans="1:4">
       <c r="A225" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B225" s="33">
         <v>348</v>
@@ -5105,7 +5105,7 @@
     </row>
     <row r="226" spans="1:4">
       <c r="A226" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B226" s="33">
         <v>349</v>
@@ -5119,7 +5119,7 @@
     </row>
     <row r="227" spans="1:4">
       <c r="A227" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B227" s="33">
         <v>718</v>
@@ -5133,7 +5133,7 @@
     </row>
     <row r="228" spans="1:4">
       <c r="A228" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B228" s="33">
         <v>720</v>
@@ -5147,7 +5147,7 @@
     </row>
     <row r="229" spans="1:4">
       <c r="A229" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B229" s="33">
         <v>723</v>
@@ -5161,7 +5161,7 @@
     </row>
     <row r="230" spans="1:4">
       <c r="A230" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B230" s="33">
         <v>724</v>
@@ -5175,7 +5175,7 @@
     </row>
     <row r="231" spans="1:4">
       <c r="A231" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B231" s="33">
         <v>794</v>
@@ -5183,7 +5183,7 @@
     </row>
     <row r="232" spans="1:4">
       <c r="A232" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B232" s="33">
         <v>795</v>
@@ -5191,7 +5191,7 @@
     </row>
     <row r="233" spans="1:4">
       <c r="A233" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B233" s="33">
         <v>796</v>
@@ -5199,7 +5199,7 @@
     </row>
     <row r="234" spans="1:4">
       <c r="A234" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B234" s="33">
         <v>797</v>
@@ -5207,7 +5207,7 @@
     </row>
     <row r="235" spans="1:4">
       <c r="A235" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B235" s="33">
         <v>798</v>
@@ -5215,7 +5215,7 @@
     </row>
     <row r="236" spans="1:4">
       <c r="A236" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B236" s="33">
         <v>799</v>
@@ -5223,7 +5223,7 @@
     </row>
     <row r="237" spans="1:4">
       <c r="A237" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B237" s="33">
         <v>726</v>
@@ -5237,7 +5237,7 @@
     </row>
     <row r="238" spans="1:4">
       <c r="A238" s="32" t="s">
-        <v>251</v>
+        <v>448</v>
       </c>
       <c r="B238" s="33">
         <v>719</v>
@@ -5251,10 +5251,10 @@
     </row>
     <row r="239" spans="1:4">
       <c r="A239" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B239" s="30" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C239" s="30">
         <v>38.074469999999998</v>
@@ -5265,10 +5265,10 @@
     </row>
     <row r="240" spans="1:4">
       <c r="A240" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B240" s="30" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C240" s="30">
         <v>38.044820000000001</v>
@@ -5279,10 +5279,10 @@
     </row>
     <row r="241" spans="1:4">
       <c r="A241" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B241" s="30" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C241" s="30">
         <v>38.121292169999997</v>
@@ -5293,10 +5293,10 @@
     </row>
     <row r="242" spans="1:4">
       <c r="A242" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B242" s="30" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C242" s="30">
         <v>38.181780430000003</v>
@@ -5307,10 +5307,10 @@
     </row>
     <row r="243" spans="1:4">
       <c r="A243" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B243" s="30" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C243" s="30">
         <v>38.043095299999997</v>
@@ -5321,10 +5321,10 @@
     </row>
     <row r="244" spans="1:4">
       <c r="A244" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B244" s="30" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C244" s="30">
         <v>38.08988506</v>
@@ -5335,10 +5335,10 @@
     </row>
     <row r="245" spans="1:4">
       <c r="A245" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B245" s="30" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C245" s="30">
         <v>38.082940000000001</v>
@@ -5349,10 +5349,10 @@
     </row>
     <row r="246" spans="1:4">
       <c r="A246" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B246" s="30" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C246" s="30">
         <v>38.259950000000003</v>
@@ -5363,10 +5363,10 @@
     </row>
     <row r="247" spans="1:4">
       <c r="A247" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B247" s="30" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C247" s="30">
         <v>38.243549999999999</v>
@@ -5377,10 +5377,10 @@
     </row>
     <row r="248" spans="1:4">
       <c r="A248" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B248" s="30" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C248" s="30">
         <v>38.242464470000002</v>
@@ -5391,10 +5391,10 @@
     </row>
     <row r="249" spans="1:4">
       <c r="A249" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B249" s="30" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C249" s="30">
         <v>38.258112920000002</v>
@@ -5405,10 +5405,10 @@
     </row>
     <row r="250" spans="1:4">
       <c r="A250" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B250" s="30" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C250" s="30">
         <v>38.042189569999998</v>
@@ -5419,10 +5419,10 @@
     </row>
     <row r="251" spans="1:4">
       <c r="A251" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B251" s="30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C251" s="30">
         <v>38.265309999999999</v>
@@ -5433,10 +5433,10 @@
     </row>
     <row r="252" spans="1:4">
       <c r="A252" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B252" s="30" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C252" s="30">
         <v>38.267819490000001</v>
@@ -5447,10 +5447,10 @@
     </row>
     <row r="253" spans="1:4">
       <c r="A253" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B253" s="30" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C253" s="30">
         <v>38.263213780000001</v>
@@ -5461,10 +5461,10 @@
     </row>
     <row r="254" spans="1:4">
       <c r="A254" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B254" s="30" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C254" s="30">
         <v>38.180309999999999</v>
@@ -5475,10 +5475,10 @@
     </row>
     <row r="255" spans="1:4">
       <c r="A255" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B255" s="30" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C255" s="30">
         <v>38.182479999999998</v>
@@ -5489,10 +5489,10 @@
     </row>
     <row r="256" spans="1:4">
       <c r="A256" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B256" s="30" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C256" s="30">
         <v>38.039000000000001</v>
@@ -5503,10 +5503,10 @@
     </row>
     <row r="257" spans="1:4">
       <c r="A257" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B257" s="30" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C257" s="30">
         <v>38.040502709999998</v>
@@ -5517,10 +5517,10 @@
     </row>
     <row r="258" spans="1:4">
       <c r="A258" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B258" s="30" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C258" s="30">
         <v>38.038130160000001</v>
@@ -5531,10 +5531,10 @@
     </row>
     <row r="259" spans="1:4">
       <c r="A259" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B259" s="30" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C259" s="30">
         <v>38.286009999999997</v>
@@ -5545,20 +5545,20 @@
     </row>
     <row r="260" spans="1:4">
       <c r="A260" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B260" s="30" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C260" s="30"/>
       <c r="D260" s="30"/>
     </row>
     <row r="261" spans="1:4">
       <c r="A261" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B261" s="30" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C261" s="30">
         <v>38.26030111</v>
@@ -5569,10 +5569,10 @@
     </row>
     <row r="262" spans="1:4">
       <c r="A262" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B262" s="30" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C262" s="30">
         <v>38.259959870000003</v>
@@ -5583,10 +5583,10 @@
     </row>
     <row r="263" spans="1:4">
       <c r="A263" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B263" s="30" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C263" s="30">
         <v>38.083607880000002</v>
@@ -5597,10 +5597,10 @@
     </row>
     <row r="264" spans="1:4">
       <c r="A264" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B264" s="30" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C264" s="30">
         <v>38.10404278</v>
@@ -5611,10 +5611,10 @@
     </row>
     <row r="265" spans="1:4">
       <c r="A265" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B265" s="30" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C265" s="30">
         <v>38.09872661</v>
@@ -5625,10 +5625,10 @@
     </row>
     <row r="266" spans="1:4">
       <c r="A266" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B266" s="30" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C266" s="30">
         <v>38.096895789999998</v>
@@ -5639,10 +5639,10 @@
     </row>
     <row r="267" spans="1:4">
       <c r="A267" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B267" s="30" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C267" s="30">
         <v>38.085120000000003</v>
@@ -5653,10 +5653,10 @@
     </row>
     <row r="268" spans="1:4">
       <c r="A268" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B268" s="30" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C268" s="30">
         <v>38.023244210000001</v>
@@ -5667,10 +5667,10 @@
     </row>
     <row r="269" spans="1:4">
       <c r="A269" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B269" s="30" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C269" s="30">
         <v>38.021912989999997</v>
@@ -5681,10 +5681,10 @@
     </row>
     <row r="270" spans="1:4">
       <c r="A270" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B270" s="30" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C270" s="30">
         <v>38.022789410000001</v>
@@ -5695,10 +5695,10 @@
     </row>
     <row r="271" spans="1:4">
       <c r="A271" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B271" s="30" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C271" s="30">
         <v>38.021887560000003</v>
@@ -5709,10 +5709,10 @@
     </row>
     <row r="272" spans="1:4">
       <c r="A272" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B272" s="30" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C272" s="30">
         <v>38.023757349999997</v>
@@ -5723,10 +5723,10 @@
     </row>
     <row r="273" spans="1:4">
       <c r="A273" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B273" s="30" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C273" s="30">
         <v>38.024821000000003</v>
@@ -5737,10 +5737,10 @@
     </row>
     <row r="274" spans="1:4">
       <c r="A274" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B274" s="30" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C274" s="30">
         <v>38.295859999999998</v>
@@ -5751,10 +5751,10 @@
     </row>
     <row r="275" spans="1:4">
       <c r="A275" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B275" s="30" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C275" s="30">
         <v>38.296002000000001</v>
@@ -5765,10 +5765,10 @@
     </row>
     <row r="276" spans="1:4">
       <c r="A276" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B276" s="30" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C276" s="30">
         <v>38.364139999999999</v>
@@ -5779,10 +5779,10 @@
     </row>
     <row r="277" spans="1:4">
       <c r="A277" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B277" s="30" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C277" s="30">
         <v>38.03228</v>
@@ -5793,10 +5793,10 @@
     </row>
     <row r="278" spans="1:4">
       <c r="A278" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B278" s="30" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C278" s="30">
         <v>38.082587820000001</v>
@@ -5807,10 +5807,10 @@
     </row>
     <row r="279" spans="1:4">
       <c r="A279" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B279" s="30" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C279" s="30">
         <v>38.084034219999999</v>
@@ -5821,10 +5821,10 @@
     </row>
     <row r="280" spans="1:4">
       <c r="A280" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B280" s="30" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C280" s="30">
         <v>38.099297280000002</v>
@@ -5835,10 +5835,10 @@
     </row>
     <row r="281" spans="1:4">
       <c r="A281" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B281" s="30" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C281" s="30">
         <v>38.303673269999997</v>
@@ -5849,10 +5849,10 @@
     </row>
     <row r="282" spans="1:4">
       <c r="A282" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B282" s="30" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C282" s="30">
         <v>38.277729919999999</v>
@@ -5863,10 +5863,10 @@
     </row>
     <row r="283" spans="1:4">
       <c r="A283" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B283" s="30" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C283" s="30">
         <v>38.242040000000003</v>
@@ -5877,10 +5877,10 @@
     </row>
     <row r="284" spans="1:4">
       <c r="A284" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B284" s="30" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C284" s="30">
         <v>38.277189999999997</v>
@@ -5891,10 +5891,10 @@
     </row>
     <row r="285" spans="1:4">
       <c r="A285" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B285" s="30" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C285" s="30">
         <v>38.246361999999998</v>
@@ -5905,10 +5905,10 @@
     </row>
     <row r="286" spans="1:4">
       <c r="A286" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B286" s="30" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C286" s="30">
         <v>38.269292</v>
@@ -5919,10 +5919,10 @@
     </row>
     <row r="287" spans="1:4">
       <c r="A287" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B287" s="30" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C287" s="30">
         <v>38.255043000000001</v>
@@ -5933,10 +5933,10 @@
     </row>
     <row r="288" spans="1:4">
       <c r="A288" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B288" s="30" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C288" s="30">
         <v>38.257888000000001</v>
@@ -5947,10 +5947,10 @@
     </row>
     <row r="289" spans="1:4">
       <c r="A289" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B289" s="30" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C289" s="30">
         <v>38.265140000000002</v>
@@ -5961,10 +5961,10 @@
     </row>
     <row r="290" spans="1:4">
       <c r="A290" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B290" s="30" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C290" s="30">
         <v>38.252679999999998</v>
@@ -5975,10 +5975,10 @@
     </row>
     <row r="291" spans="1:4">
       <c r="A291" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B291" s="30" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C291" s="30">
         <v>38.273775000000001</v>
@@ -5989,10 +5989,10 @@
     </row>
     <row r="292" spans="1:4">
       <c r="A292" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B292" s="30" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C292" s="30">
         <v>38.244607000000002</v>
@@ -6003,10 +6003,10 @@
     </row>
     <row r="293" spans="1:4">
       <c r="A293" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B293" s="30" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C293" s="30">
         <v>38.282319999999999</v>
@@ -6017,10 +6017,10 @@
     </row>
     <row r="294" spans="1:4">
       <c r="A294" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B294" s="30" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C294" s="30">
         <v>38.284170000000003</v>
@@ -6031,10 +6031,10 @@
     </row>
     <row r="295" spans="1:4">
       <c r="A295" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B295" s="30" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C295" s="30">
         <v>38.288989999999998</v>
@@ -6045,10 +6045,10 @@
     </row>
     <row r="296" spans="1:4">
       <c r="A296" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B296" s="30" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C296" s="30">
         <v>38.287590000000002</v>
@@ -6059,10 +6059,10 @@
     </row>
     <row r="297" spans="1:4">
       <c r="A297" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B297" s="30" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C297" s="30">
         <v>38.29607</v>
@@ -6073,10 +6073,10 @@
     </row>
     <row r="298" spans="1:4">
       <c r="A298" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B298" s="30" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C298" s="30">
         <v>38.278500000000001</v>
@@ -6087,10 +6087,10 @@
     </row>
     <row r="299" spans="1:4">
       <c r="A299" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B299" s="30" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C299" s="30">
         <v>38.290030000000002</v>
@@ -6101,10 +6101,10 @@
     </row>
     <row r="300" spans="1:4">
       <c r="A300" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B300" s="30" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C300" s="30">
         <v>38.296169999999996</v>
@@ -6115,10 +6115,10 @@
     </row>
     <row r="301" spans="1:4">
       <c r="A301" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B301" s="30" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C301" s="30">
         <v>38.269620000000003</v>
@@ -6129,10 +6129,10 @@
     </row>
     <row r="302" spans="1:4">
       <c r="A302" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B302" s="30" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C302" s="30">
         <v>38.275649999999999</v>
@@ -6143,10 +6143,10 @@
     </row>
     <row r="303" spans="1:4">
       <c r="A303" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B303" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C303" s="30">
         <v>38.249670000000002</v>
@@ -6157,10 +6157,10 @@
     </row>
     <row r="304" spans="1:4">
       <c r="A304" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B304" s="30" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C304" s="30">
         <v>38.247709999999998</v>
@@ -6171,10 +6171,10 @@
     </row>
     <row r="305" spans="1:4">
       <c r="A305" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B305" s="30" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C305" s="30">
         <v>38.26238</v>
@@ -6185,10 +6185,10 @@
     </row>
     <row r="306" spans="1:4">
       <c r="A306" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B306" s="30" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C306" s="30">
         <v>38.267040000000001</v>
@@ -6199,10 +6199,10 @@
     </row>
     <row r="307" spans="1:4">
       <c r="A307" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B307" s="30" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C307" s="30">
         <v>38.258663110000001</v>
@@ -6213,10 +6213,10 @@
     </row>
     <row r="308" spans="1:4">
       <c r="A308" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B308" s="30" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C308" s="30">
         <v>38.259518229999998</v>
@@ -6227,10 +6227,10 @@
     </row>
     <row r="309" spans="1:4">
       <c r="A309" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B309" s="30" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C309" s="30">
         <v>38.259779999999999</v>
@@ -6241,10 +6241,10 @@
     </row>
     <row r="310" spans="1:4">
       <c r="A310" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B310" s="30" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C310" s="30">
         <v>38.25902</v>
@@ -6255,10 +6255,10 @@
     </row>
     <row r="311" spans="1:4">
       <c r="A311" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B311" s="30" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C311" s="30">
         <v>38.260269030000003</v>
@@ -6269,10 +6269,10 @@
     </row>
     <row r="312" spans="1:4">
       <c r="A312" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B312" s="30" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C312" s="30">
         <v>38.258149009999997</v>
@@ -6283,10 +6283,10 @@
     </row>
     <row r="313" spans="1:4">
       <c r="A313" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B313" s="30" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C313" s="30">
         <v>38.249980829999998</v>
@@ -6297,10 +6297,10 @@
     </row>
     <row r="314" spans="1:4">
       <c r="A314" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B314" s="30" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C314" s="30">
         <v>38.242319999999999</v>
@@ -6311,10 +6311,10 @@
     </row>
     <row r="315" spans="1:4">
       <c r="A315" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B315" s="30" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C315" s="30">
         <v>38.256869999999999</v>
@@ -6325,10 +6325,10 @@
     </row>
     <row r="316" spans="1:4">
       <c r="A316" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B316" s="30" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C316" s="30">
         <v>38.234140869999997</v>
@@ -6339,10 +6339,10 @@
     </row>
     <row r="317" spans="1:4">
       <c r="A317" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B317" s="30" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C317" s="30">
         <v>38.24640849</v>
@@ -6353,10 +6353,10 @@
     </row>
     <row r="318" spans="1:4">
       <c r="A318" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B318" s="30" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C318" s="30">
         <v>38.263632440000002</v>
@@ -6367,10 +6367,10 @@
     </row>
     <row r="319" spans="1:4">
       <c r="A319" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B319" s="30" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C319" s="30">
         <v>38.279973130000002</v>
@@ -6381,10 +6381,10 @@
     </row>
     <row r="320" spans="1:4">
       <c r="A320" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B320" s="30" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C320" s="30">
         <v>38.291833349999997</v>
@@ -6395,10 +6395,10 @@
     </row>
     <row r="321" spans="1:4">
       <c r="A321" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B321" s="30" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C321" s="30">
         <v>38.192741210000001</v>
@@ -6409,10 +6409,10 @@
     </row>
     <row r="322" spans="1:4">
       <c r="A322" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B322" s="30" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C322" s="30">
         <v>38.293072469999998</v>
@@ -6423,10 +6423,10 @@
     </row>
     <row r="323" spans="1:4">
       <c r="A323" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B323" s="30" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C323" s="30">
         <v>38.24394144</v>
@@ -6437,10 +6437,10 @@
     </row>
     <row r="324" spans="1:4">
       <c r="A324" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B324" s="30" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C324" s="30">
         <v>38.31306549</v>
@@ -6451,10 +6451,10 @@
     </row>
     <row r="325" spans="1:4">
       <c r="A325" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B325" s="30" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C325" s="30">
         <v>38.081829999999997</v>
@@ -6465,10 +6465,10 @@
     </row>
     <row r="326" spans="1:4">
       <c r="A326" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B326" s="30" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C326" s="30">
         <v>38.083069999999999</v>
@@ -6479,10 +6479,10 @@
     </row>
     <row r="327" spans="1:4">
       <c r="A327" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B327" s="30" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C327" s="30">
         <v>38.08558</v>
@@ -6493,10 +6493,10 @@
     </row>
     <row r="328" spans="1:4">
       <c r="A328" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B328" s="30" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C328" s="30">
         <v>38.08766</v>
@@ -6507,10 +6507,10 @@
     </row>
     <row r="329" spans="1:4">
       <c r="A329" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B329" s="30" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C329" s="30">
         <v>38.10013</v>
@@ -6521,10 +6521,10 @@
     </row>
     <row r="330" spans="1:4">
       <c r="A330" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B330" s="30" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C330" s="30">
         <v>38.100540000000002</v>
@@ -6535,10 +6535,10 @@
     </row>
     <row r="331" spans="1:4">
       <c r="A331" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B331" s="30" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C331" s="30">
         <v>38.080979999999997</v>
@@ -6549,10 +6549,10 @@
     </row>
     <row r="332" spans="1:4">
       <c r="A332" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B332" s="30" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C332" s="30">
         <v>38.085477750000003</v>
@@ -6563,10 +6563,10 @@
     </row>
     <row r="333" spans="1:4">
       <c r="A333" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B333" s="30" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C333" s="30">
         <v>38.083220560000001</v>
@@ -6577,10 +6577,10 @@
     </row>
     <row r="334" spans="1:4">
       <c r="A334" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B334" s="30" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C334" s="30">
         <v>38.077246090000003</v>
@@ -6591,10 +6591,10 @@
     </row>
     <row r="335" spans="1:4">
       <c r="A335" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B335" s="30" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C335" s="30">
         <v>38.077816849999998</v>
@@ -6605,10 +6605,10 @@
     </row>
     <row r="336" spans="1:4">
       <c r="A336" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B336" s="30" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C336" s="30">
         <v>38.259108210000001</v>
@@ -6619,10 +6619,10 @@
     </row>
     <row r="337" spans="1:4">
       <c r="A337" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B337" s="30" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C337" s="30">
         <v>38.279969999999999</v>
@@ -6633,10 +6633,10 @@
     </row>
     <row r="338" spans="1:4">
       <c r="A338" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B338" s="30" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C338" s="30">
         <v>38.309820799999997</v>
@@ -6647,10 +6647,10 @@
     </row>
     <row r="339" spans="1:4">
       <c r="A339" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B339" s="30" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C339" s="30">
         <v>38.278499140000001</v>
@@ -6661,10 +6661,10 @@
     </row>
     <row r="340" spans="1:4">
       <c r="A340" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B340" s="30" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C340" s="30">
         <v>38.032170000000001</v>
@@ -6675,10 +6675,10 @@
     </row>
     <row r="341" spans="1:4">
       <c r="A341" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B341" s="30" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C341" s="30">
         <v>38.03201</v>
@@ -6689,10 +6689,10 @@
     </row>
     <row r="342" spans="1:4">
       <c r="A342" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B342" s="30" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C342" s="30">
         <v>38.009160000000001</v>
@@ -6703,10 +6703,10 @@
     </row>
     <row r="343" spans="1:4">
       <c r="A343" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B343" s="30" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C343" s="30">
         <v>38.008040000000001</v>
@@ -6717,10 +6717,10 @@
     </row>
     <row r="344" spans="1:4">
       <c r="A344" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B344" s="30" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C344" s="30">
         <v>38.003909999999998</v>
@@ -6731,10 +6731,10 @@
     </row>
     <row r="345" spans="1:4">
       <c r="A345" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B345" s="30" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C345" s="30">
         <v>38.003450000000001</v>
@@ -6745,10 +6745,10 @@
     </row>
     <row r="346" spans="1:4">
       <c r="A346" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B346" s="30" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C346" s="30">
         <v>37.997709999999998</v>
@@ -6759,10 +6759,10 @@
     </row>
     <row r="347" spans="1:4">
       <c r="A347" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B347" s="30" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C347" s="30">
         <v>37.997520000000002</v>
@@ -6773,10 +6773,10 @@
     </row>
     <row r="348" spans="1:4">
       <c r="A348" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B348" s="30" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C348" s="30">
         <v>38.249240190000002</v>
@@ -6787,10 +6787,10 @@
     </row>
     <row r="349" spans="1:4">
       <c r="A349" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B349" s="30" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C349" s="30">
         <v>38.244989259999997</v>
@@ -6801,10 +6801,10 @@
     </row>
     <row r="350" spans="1:4">
       <c r="A350" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B350" s="30" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C350" s="30">
         <v>38.238947359999997</v>
@@ -6815,10 +6815,10 @@
     </row>
     <row r="351" spans="1:4">
       <c r="A351" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B351" s="30" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C351" s="30">
         <v>38.251475419999998</v>
@@ -6829,10 +6829,10 @@
     </row>
     <row r="352" spans="1:4">
       <c r="A352" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B352" s="30" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C352" s="30">
         <v>38.24192</v>
@@ -6843,10 +6843,10 @@
     </row>
     <row r="353" spans="1:4">
       <c r="A353" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B353" s="30" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C353" s="30">
         <v>38.237220000000001</v>
@@ -6857,10 +6857,10 @@
     </row>
     <row r="354" spans="1:4">
       <c r="A354" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B354" s="30" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C354" s="30">
         <v>38.245260629999997</v>
@@ -6871,20 +6871,20 @@
     </row>
     <row r="355" spans="1:4">
       <c r="A355" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B355" s="30" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C355" s="30"/>
       <c r="D355" s="30"/>
     </row>
     <row r="356" spans="1:4">
       <c r="A356" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B356" s="30" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C356" s="30">
         <v>38.094700000000003</v>
@@ -6895,10 +6895,10 @@
     </row>
     <row r="357" spans="1:4">
       <c r="A357" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B357" s="30" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C357" s="30">
         <v>38.326660760000003</v>
@@ -6909,10 +6909,10 @@
     </row>
     <row r="358" spans="1:4">
       <c r="A358" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B358" s="30" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C358" s="30">
         <v>38.333898980000001</v>
@@ -6923,10 +6923,10 @@
     </row>
     <row r="359" spans="1:4">
       <c r="A359" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B359" s="30" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C359" s="30">
         <v>38.344457859999999</v>
@@ -6937,10 +6937,10 @@
     </row>
     <row r="360" spans="1:4">
       <c r="A360" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B360" s="30" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C360" s="30">
         <v>38.299759999999999</v>
@@ -6951,10 +6951,10 @@
     </row>
     <row r="361" spans="1:4">
       <c r="A361" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B361" s="30" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C361" s="30">
         <v>38.299639999999997</v>
@@ -6965,10 +6965,10 @@
     </row>
     <row r="362" spans="1:4">
       <c r="A362" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B362" s="30" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C362" s="30">
         <v>38.261318639999999</v>
@@ -6979,10 +6979,10 @@
     </row>
     <row r="363" spans="1:4">
       <c r="A363" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B363" s="30" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C363" s="30">
         <v>38.169350000000001</v>
@@ -6993,10 +6993,10 @@
     </row>
     <row r="364" spans="1:4">
       <c r="A364" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B364" s="30" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C364" s="30">
         <v>38.356349690000002</v>
@@ -7007,10 +7007,10 @@
     </row>
     <row r="365" spans="1:4">
       <c r="A365" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B365" s="30" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C365" s="30">
         <v>38.120756800000002</v>
@@ -7021,10 +7021,10 @@
     </row>
     <row r="366" spans="1:4">
       <c r="A366" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B366" s="30" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C366" s="30">
         <v>38.122772070000003</v>
@@ -7035,10 +7035,10 @@
     </row>
     <row r="367" spans="1:4">
       <c r="A367" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B367" s="30" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C367" s="30">
         <v>38.128327800000001</v>
@@ -7049,10 +7049,10 @@
     </row>
     <row r="368" spans="1:4">
       <c r="A368" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B368" s="30" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C368" s="30">
         <v>38.134869999999999</v>
@@ -7063,10 +7063,10 @@
     </row>
     <row r="369" spans="1:4">
       <c r="A369" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B369" s="30" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C369" s="30">
         <v>38.134869999999999</v>
@@ -7077,10 +7077,10 @@
     </row>
     <row r="370" spans="1:4">
       <c r="A370" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B370" s="30" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C370" s="30">
         <v>38.113599999999998</v>
@@ -7091,10 +7091,10 @@
     </row>
     <row r="371" spans="1:4">
       <c r="A371" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B371" s="30" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C371" s="30">
         <v>38.113779999999998</v>
@@ -7105,10 +7105,10 @@
     </row>
     <row r="372" spans="1:4">
       <c r="A372" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B372" s="30" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C372" s="30">
         <v>38.09502792</v>
@@ -7119,10 +7119,10 @@
     </row>
     <row r="373" spans="1:4">
       <c r="A373" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B373" s="30" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C373" s="30">
         <v>38.334020000000002</v>
@@ -7133,10 +7133,10 @@
     </row>
     <row r="374" spans="1:4">
       <c r="A374" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B374" s="30" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C374" s="30">
         <v>38.045928529999998</v>
@@ -7147,10 +7147,10 @@
     </row>
     <row r="375" spans="1:4">
       <c r="A375" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B375" s="30" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C375" s="30">
         <v>38.226939999999999</v>
@@ -7161,10 +7161,10 @@
     </row>
     <row r="376" spans="1:4">
       <c r="A376" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B376" s="30" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C376" s="30">
         <v>38.226010000000002</v>
@@ -7175,10 +7175,10 @@
     </row>
     <row r="377" spans="1:4">
       <c r="A377" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B377" s="30" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C377" s="30">
         <v>38.049653829999997</v>
@@ -7189,10 +7189,10 @@
     </row>
     <row r="378" spans="1:4">
       <c r="A378" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B378" s="30" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C378" s="30">
         <v>38.037943380000002</v>
@@ -7203,10 +7203,10 @@
     </row>
     <row r="379" spans="1:4">
       <c r="A379" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B379" s="30" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C379" s="30">
         <v>38.030609779999999</v>
@@ -7217,10 +7217,10 @@
     </row>
     <row r="380" spans="1:4">
       <c r="A380" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B380" s="30" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C380" s="30">
         <v>38.052289080000001</v>
@@ -7231,10 +7231,10 @@
     </row>
     <row r="381" spans="1:4">
       <c r="A381" s="28" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B381" s="30" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C381" s="30">
         <v>38.052123680000001</v>
@@ -7245,10 +7245,10 @@
     </row>
     <row r="382" spans="1:4">
       <c r="A382" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B382" s="34" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C382" s="36">
         <v>38.544499999999999</v>
@@ -7259,10 +7259,10 @@
     </row>
     <row r="383" spans="1:4">
       <c r="A383" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B383" s="35" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C383" s="37">
         <v>38.528060000000004</v>
@@ -7273,10 +7273,10 @@
     </row>
     <row r="384" spans="1:4">
       <c r="A384" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B384" s="35" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C384" s="37">
         <v>38.518500000000003</v>
@@ -7287,10 +7287,10 @@
     </row>
     <row r="385" spans="1:4">
       <c r="A385" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B385" s="35" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C385" s="37">
         <v>38.494390000000003</v>
@@ -7301,10 +7301,10 @@
     </row>
     <row r="386" spans="1:4">
       <c r="A386" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B386" s="35" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C386" s="37">
         <v>38.436971</v>
@@ -7315,10 +7315,10 @@
     </row>
     <row r="387" spans="1:4">
       <c r="A387" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B387" s="35" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C387" s="37">
         <v>38.466810000000002</v>
@@ -7329,10 +7329,10 @@
     </row>
     <row r="388" spans="1:4">
       <c r="A388" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B388" s="35" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C388" s="37">
         <v>38.431890000000003</v>
@@ -7343,10 +7343,10 @@
     </row>
     <row r="389" spans="1:4">
       <c r="A389" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B389" s="35" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C389" s="37">
         <v>38.389389999999999</v>
@@ -7357,10 +7357,10 @@
     </row>
     <row r="390" spans="1:4">
       <c r="A390" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B390" s="35" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C390" s="37">
         <v>38.354959999999998</v>
@@ -7371,10 +7371,10 @@
     </row>
     <row r="391" spans="1:4">
       <c r="A391" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B391" s="35" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C391" s="37">
         <v>38.274279999999997</v>
@@ -7385,10 +7385,10 @@
     </row>
     <row r="392" spans="1:4">
       <c r="A392" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B392" s="35" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C392" s="37">
         <v>38.282465000000002</v>
@@ -7399,10 +7399,10 @@
     </row>
     <row r="393" spans="1:4">
       <c r="A393" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B393" s="35" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C393" s="38">
         <v>38.355609999999999</v>
@@ -7413,10 +7413,10 @@
     </row>
     <row r="394" spans="1:4">
       <c r="A394" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B394" s="35" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C394" s="38">
         <v>38.364699999999999</v>
@@ -7427,10 +7427,10 @@
     </row>
     <row r="395" spans="1:4">
       <c r="A395" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B395" s="35" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C395" s="38">
         <v>38.371920000000003</v>
@@ -7441,10 +7441,10 @@
     </row>
     <row r="396" spans="1:4">
       <c r="A396" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B396" s="35" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C396" s="38">
         <v>38.382579999999997</v>
@@ -7455,30 +7455,30 @@
     </row>
     <row r="397" spans="1:4">
       <c r="A397" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B397" s="35" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C397" s="39"/>
       <c r="D397" s="39"/>
     </row>
     <row r="398" spans="1:4">
       <c r="A398" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B398" s="35" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C398" s="40"/>
       <c r="D398" s="40"/>
     </row>
     <row r="399" spans="1:4">
       <c r="A399" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B399" s="35" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C399" s="36">
         <v>38.675919999999998</v>
@@ -7489,10 +7489,10 @@
     </row>
     <row r="400" spans="1:4">
       <c r="A400" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B400" s="35" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C400" s="37">
         <v>38.749789999999997</v>
@@ -7503,10 +7503,10 @@
     </row>
     <row r="401" spans="1:4">
       <c r="A401" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B401" s="35" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C401" s="37">
         <v>38.474170000000001</v>
@@ -7517,10 +7517,10 @@
     </row>
     <row r="402" spans="1:4">
       <c r="A402" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B402" s="35" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C402" s="41">
         <v>38.473550000000003</v>
@@ -7531,10 +7531,10 @@
     </row>
     <row r="403" spans="1:4">
       <c r="A403" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B403" s="35" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C403" s="37">
         <v>38.466957999999998</v>
@@ -7545,10 +7545,10 @@
     </row>
     <row r="404" spans="1:4">
       <c r="A404" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B404" s="35" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C404" s="41">
         <v>38.676366999999999</v>
@@ -7559,10 +7559,10 @@
     </row>
     <row r="405" spans="1:4">
       <c r="A405" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B405" s="35" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C405" s="42">
         <v>38.605218999999998</v>
@@ -7573,50 +7573,50 @@
     </row>
     <row r="406" spans="1:4">
       <c r="A406" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B406" s="35" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C406" s="41"/>
       <c r="D406" s="41"/>
     </row>
     <row r="407" spans="1:4">
       <c r="A407" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B407" s="35" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C407" s="44"/>
       <c r="D407" s="44"/>
     </row>
     <row r="408" spans="1:4">
       <c r="A408" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B408" s="35" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C408" s="44"/>
       <c r="D408" s="44"/>
     </row>
     <row r="409" spans="1:4">
       <c r="A409" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B409" s="35" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C409" s="41"/>
       <c r="D409" s="41"/>
     </row>
     <row r="410" spans="1:4">
       <c r="A410" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B410" s="35" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C410" s="37">
         <v>38.353383000000001</v>
@@ -7627,10 +7627,10 @@
     </row>
     <row r="411" spans="1:4">
       <c r="A411" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B411" s="35" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C411" s="37">
         <v>38.605218999999998</v>
@@ -7641,10 +7641,10 @@
     </row>
     <row r="412" spans="1:4">
       <c r="A412" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B412" s="35" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C412" s="37">
         <v>38.565379999999998</v>
@@ -7655,10 +7655,10 @@
     </row>
     <row r="413" spans="1:4">
       <c r="A413" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B413" s="35" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C413" s="37">
         <v>38.565309999999997</v>
@@ -7669,10 +7669,10 @@
     </row>
     <row r="414" spans="1:4">
       <c r="A414" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B414" s="35" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C414" s="36">
         <v>38.675919999999998</v>
@@ -7683,10 +7683,10 @@
     </row>
     <row r="415" spans="1:4">
       <c r="A415" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B415" s="35" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C415" s="39">
         <v>38.567056999999998</v>
@@ -7697,10 +7697,10 @@
     </row>
     <row r="416" spans="1:4">
       <c r="A416" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B416" s="35" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C416" s="39">
         <v>38.573110999999997</v>
@@ -7711,20 +7711,20 @@
     </row>
     <row r="417" spans="1:4">
       <c r="A417" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B417" s="35" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C417" s="39"/>
       <c r="D417" s="39"/>
     </row>
     <row r="418" spans="1:4">
       <c r="A418" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B418" s="35" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C418" s="45">
         <v>38.242100000000001</v>
@@ -7735,10 +7735,10 @@
     </row>
     <row r="419" spans="1:4">
       <c r="A419" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B419" s="35" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C419" s="37">
         <v>38.474815999999997</v>
@@ -7749,10 +7749,10 @@
     </row>
     <row r="420" spans="1:4">
       <c r="A420" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B420" s="35" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C420" s="39">
         <v>38.793456999999997</v>
@@ -7763,10 +7763,10 @@
     </row>
     <row r="421" spans="1:4">
       <c r="A421" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B421" s="35" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C421" s="42">
         <v>38.842001000000003</v>
@@ -7777,10 +7777,10 @@
     </row>
     <row r="422" spans="1:4">
       <c r="A422" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B422" s="35" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C422" s="39">
         <v>38.159737</v>
@@ -7791,10 +7791,10 @@
     </row>
     <row r="423" spans="1:4">
       <c r="A423" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B423" s="35" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C423" s="39">
         <v>38.213166999999999</v>
@@ -7805,10 +7805,10 @@
     </row>
     <row r="424" spans="1:4">
       <c r="A424" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B424" s="35" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C424" s="46">
         <v>38.093400000000003</v>
@@ -7819,10 +7819,10 @@
     </row>
     <row r="425" spans="1:4">
       <c r="A425" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B425" s="35" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C425" s="43">
         <v>38.531880999999998</v>
@@ -7833,20 +7833,20 @@
     </row>
     <row r="426" spans="1:4">
       <c r="A426" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B426" s="35" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C426" s="39"/>
       <c r="D426" s="39"/>
     </row>
     <row r="427" spans="1:4">
       <c r="A427" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B427" s="35" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C427" s="39">
         <v>38.681621</v>
@@ -7857,10 +7857,10 @@
     </row>
     <row r="428" spans="1:4">
       <c r="A428" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B428" s="35" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C428" s="43">
         <v>38.47157</v>
@@ -7871,10 +7871,10 @@
     </row>
     <row r="429" spans="1:4">
       <c r="A429" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B429" s="35" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C429" s="43">
         <v>38.470230000000001</v>
@@ -7885,10 +7885,10 @@
     </row>
     <row r="430" spans="1:4">
       <c r="A430" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B430" s="35" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C430" s="43">
         <v>38.471620000000001</v>
@@ -7899,10 +7899,10 @@
     </row>
     <row r="431" spans="1:4">
       <c r="A431" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B431" s="35" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C431" s="43">
         <v>38.472580000000001</v>

</xml_diff>